<commit_message>
Changed GS + Link Parameters
</commit_message>
<xml_diff>
--- a/Sheets/Link Budget.xlsx
+++ b/Sheets/Link Budget.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD7E671-3779-4541-98B6-5E7FFE45A04F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD05BFC1-F957-4BC7-963D-70AF8DF6E121}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
   <si>
     <t>Tx Power</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Total Noise</t>
+  </si>
+  <si>
+    <t>ADS-B to Sat</t>
   </si>
 </sst>
 </file>
@@ -578,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:AA45"/>
+  <dimension ref="B3:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N7" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,6 +856,9 @@
       <c r="J16" t="s">
         <v>4</v>
       </c>
+      <c r="M16" t="s">
+        <v>72</v>
+      </c>
       <c r="O16" t="s">
         <v>52</v>
       </c>
@@ -871,10 +877,7 @@
         <v>48</v>
       </c>
       <c r="O18">
-        <v>20</v>
-      </c>
-      <c r="R18">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="S18">
         <v>17</v>
@@ -893,9 +896,6 @@
       <c r="O19">
         <v>4.5</v>
       </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
       <c r="S19">
         <v>2.5</v>
       </c>
@@ -913,9 +913,6 @@
       <c r="O20">
         <v>-0.35</v>
       </c>
-      <c r="R20">
-        <v>-1.02</v>
-      </c>
       <c r="S20">
         <v>-1.02</v>
       </c>
@@ -933,9 +930,6 @@
       <c r="O21">
         <v>1090</v>
       </c>
-      <c r="R21">
-        <v>433</v>
-      </c>
       <c r="S21">
         <v>433</v>
       </c>
@@ -948,19 +942,16 @@
         <v>48</v>
       </c>
       <c r="M22">
-        <v>408</v>
+        <v>645</v>
       </c>
       <c r="O22">
-        <v>408</v>
-      </c>
-      <c r="R22">
-        <v>408</v>
+        <v>645</v>
       </c>
       <c r="S22">
-        <v>408</v>
+        <v>645</v>
       </c>
       <c r="V22">
-        <v>408</v>
+        <v>645</v>
       </c>
     </row>
     <row r="23" spans="10:23" x14ac:dyDescent="0.25">
@@ -971,13 +962,10 @@
         <v>4.5</v>
       </c>
       <c r="O23">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="R23">
-        <v>16.899999999999999</v>
+        <v>15</v>
       </c>
       <c r="S23">
-        <v>16.899999999999999</v>
+        <v>15</v>
       </c>
       <c r="V23">
         <v>2</v>
@@ -993,9 +981,6 @@
       <c r="O24">
         <v>-0.40899999999999997</v>
       </c>
-      <c r="R24">
-        <v>-0.40899999999999997</v>
-      </c>
       <c r="S24">
         <v>-0.40899999999999997</v>
       </c>
@@ -1013,9 +998,6 @@
       <c r="O25">
         <v>320</v>
       </c>
-      <c r="R25">
-        <v>320</v>
-      </c>
       <c r="S25">
         <v>320</v>
       </c>
@@ -1033,9 +1015,6 @@
       <c r="O26">
         <v>2000</v>
       </c>
-      <c r="R26">
-        <v>25</v>
-      </c>
       <c r="S26">
         <v>25</v>
       </c>
@@ -1061,10 +1040,7 @@
       <c r="P27" t="s">
         <v>56</v>
       </c>
-      <c r="R27" s="3">
-        <f>10*LOG10(370/290+1)</f>
-        <v>3.571459376429126</v>
-      </c>
+      <c r="R27" s="3"/>
       <c r="S27" s="3">
         <f>10*LOG10(370/290+1)</f>
         <v>3.571459376429126</v>
@@ -1080,32 +1056,28 @@
       </c>
       <c r="M28">
         <f>20*LOG10(M22*1000)+20*LOG10(M21*1000000)+20*LOG10(4*PI()/(300000000))</f>
-        <v>145.40350540665878</v>
+        <v>149.38149643756651</v>
       </c>
       <c r="N28" t="s">
         <v>56</v>
       </c>
       <c r="O28">
         <f>20*LOG10(O22*1000)+20*LOG10(O21*1000000)+20*LOG10(4*PI()/(300000000))</f>
-        <v>145.40350540665878</v>
+        <v>149.38149643756651</v>
       </c>
       <c r="P28" t="s">
         <v>56</v>
-      </c>
-      <c r="R28">
-        <f>20*LOG10(R22*1000)+20*LOG10(R21*1000000)+20*LOG10(4*PI()/(300000000))</f>
-        <v>137.38473337491359</v>
       </c>
       <c r="S28">
         <f>20*LOG10(S22*1000)+20*LOG10(S21*1000000)+20*LOG10(4*PI()/(300000000))</f>
-        <v>137.38473337491359</v>
+        <v>141.36272440582133</v>
       </c>
       <c r="T28" t="s">
         <v>56</v>
       </c>
       <c r="V28">
         <f>20*LOG10(V22*1000)+20*LOG10(V21*1000000)+20*LOG10(4*PI()/(300000000))</f>
-        <v>137.38473337491359</v>
+        <v>141.36272440582133</v>
       </c>
       <c r="W28" t="s">
         <v>56</v>
@@ -1117,32 +1089,28 @@
       </c>
       <c r="M29">
         <f>M18+M19+M20-M28+M23+M24-M27</f>
-        <v>-91.423505406658776</v>
+        <v>-95.401496437566507</v>
       </c>
       <c r="N29" t="s">
         <v>55</v>
       </c>
       <c r="O29">
         <f>O18+O19+O20-O28+O23+O24</f>
-        <v>-104.76250540665878</v>
+        <v>-100.64049643756651</v>
       </c>
       <c r="P29" t="s">
         <v>55</v>
       </c>
-      <c r="R29">
-        <f>R18+R19+R20-R28+R23+R24-R27</f>
-        <v>-105.48519275134274</v>
-      </c>
       <c r="S29">
         <f>S18+S19+S20-S28+S23+S24-S27</f>
-        <v>-105.98519275134274</v>
+        <v>-111.86318378225046</v>
       </c>
       <c r="T29" t="s">
         <v>55</v>
       </c>
       <c r="V29">
         <f>V18+V19+V20-V28+V23+V24-V27</f>
-        <v>-75.863733374913593</v>
+        <v>-79.841724405821324</v>
       </c>
       <c r="W29" t="s">
         <v>55</v>
@@ -1166,10 +1134,7 @@
       <c r="P30" t="s">
         <v>55</v>
       </c>
-      <c r="R30" s="3">
-        <f>10*LOG10($AA$4*$L$7*$P$13*1000*1000)</f>
-        <v>-129.84745058029668</v>
-      </c>
+      <c r="R30" s="3"/>
       <c r="S30" s="3">
         <f>10*LOG10($AA$4*$L$7*$P$13*1000*1000)</f>
         <v>-129.84745058029668</v>
@@ -1198,10 +1163,7 @@
         <f>O30+O27</f>
         <v>-107.24509133394811</v>
       </c>
-      <c r="R31" s="3">
-        <f>R30+R27</f>
-        <v>-126.27599120386755</v>
-      </c>
+      <c r="R31" s="3"/>
       <c r="S31" s="3">
         <f>S30+S27</f>
         <v>-126.27599120386755</v>
@@ -1217,32 +1179,29 @@
       </c>
       <c r="M32" s="3">
         <f>M29-M31</f>
-        <v>19.903345260358279</v>
+        <v>15.925354229450548</v>
       </c>
       <c r="N32" t="s">
         <v>56</v>
       </c>
       <c r="O32" s="3">
         <f>O29-O31</f>
-        <v>2.4825859272893354</v>
+        <v>6.6045948963815988</v>
       </c>
       <c r="P32" t="s">
         <v>56</v>
       </c>
-      <c r="R32" s="3">
-        <f>R29-R31</f>
-        <v>20.790798452524811</v>
-      </c>
+      <c r="R32" s="3"/>
       <c r="S32" s="3">
         <f>S29-S31</f>
-        <v>20.290798452524811</v>
+        <v>14.412807421617089</v>
       </c>
       <c r="T32" t="s">
         <v>56</v>
       </c>
       <c r="V32" s="3">
         <f>V29-V31</f>
-        <v>50.183717205383076</v>
+        <v>46.205726174475345</v>
       </c>
       <c r="W32" t="s">
         <v>56</v>
@@ -1259,10 +1218,6 @@
       <c r="O34">
         <f>2^($L11*1000000/($L13*1000))-1</f>
         <v>0.41421356237309515</v>
-      </c>
-      <c r="R34">
-        <f>2^($P11/($P$13*1000))-1</f>
-        <v>0.3049549476889577</v>
       </c>
       <c r="S34">
         <f>2^($P11/($P$13*1000))-1</f>
@@ -1291,10 +1246,6 @@
       <c r="P35" t="s">
         <v>56</v>
       </c>
-      <c r="R35">
-        <f>10*LOG10(R34)</f>
-        <v>-5.1576431611319489</v>
-      </c>
       <c r="S35">
         <f>10*LOG10(S34)</f>
         <v>-5.1576431611319489</v>
@@ -1316,32 +1267,28 @@
       </c>
       <c r="M37">
         <f>M32-M35</f>
-        <v>23.73110211373691</v>
+        <v>19.753111082829179</v>
       </c>
       <c r="N37" t="s">
         <v>56</v>
       </c>
       <c r="O37">
         <f>O32-O35</f>
-        <v>6.3103427806679653</v>
+        <v>10.43235174976023</v>
       </c>
       <c r="P37" t="s">
         <v>56</v>
-      </c>
-      <c r="R37">
-        <f>R32-R35</f>
-        <v>25.948441613656762</v>
       </c>
       <c r="S37">
         <f>S32-S35</f>
-        <v>25.448441613656762</v>
+        <v>19.570450582749039</v>
       </c>
       <c r="T37" t="s">
         <v>56</v>
       </c>
       <c r="V37">
         <f>V32-V35</f>
-        <v>55.341360366515026</v>
+        <v>51.363369335607295</v>
       </c>
       <c r="W37" t="s">
         <v>56</v>
@@ -1359,10 +1306,6 @@
         <f>$L11*1000000</f>
         <v>1000000</v>
       </c>
-      <c r="R39">
-        <f>$P11</f>
-        <v>9600</v>
-      </c>
       <c r="S39">
         <f>$P11</f>
         <v>9600</v>
@@ -1378,32 +1321,28 @@
       </c>
       <c r="M41">
         <f>M32+10*LOG10($L13*1000/(M39))</f>
-        <v>22.913645216998091</v>
+        <v>18.93565418609036</v>
       </c>
       <c r="N41" t="s">
         <v>56</v>
       </c>
       <c r="O41">
         <f>O32+10*LOG10($L13*1000/(O39))</f>
-        <v>5.4928858839291479</v>
+        <v>9.6148948530214113</v>
       </c>
       <c r="P41" t="s">
         <v>56</v>
-      </c>
-      <c r="R41">
-        <f>R32+10*LOG10($P13*1000/(R39))</f>
-        <v>24.947486208849504</v>
       </c>
       <c r="S41">
         <f>S32+10*LOG10($P13*1000/(S39))</f>
-        <v>24.447486208849504</v>
+        <v>18.569495177941782</v>
       </c>
       <c r="T41" t="s">
         <v>56</v>
       </c>
       <c r="V41">
         <f>V32+10*LOG10($P13*1000/(V39))</f>
-        <v>54.340404961707769</v>
+        <v>50.362413930800038</v>
       </c>
       <c r="W41" t="s">
         <v>56</v>
@@ -1414,11 +1353,6 @@
     </row>
     <row r="44" spans="10:23" x14ac:dyDescent="0.25">
       <c r="M44" s="3"/>
-    </row>
-    <row r="45" spans="10:23" x14ac:dyDescent="0.25">
-      <c r="K45">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Modified Link Budget, added some pics
</commit_message>
<xml_diff>
--- a/Sheets/Link Budget.xlsx
+++ b/Sheets/Link Budget.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC878582-E268-440B-AA8E-7732DBA0CE63}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4E5932-D3AD-44A7-ACBD-9C9B43A6A21C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>Tx Power</t>
   </si>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +883,7 @@
         <v>17</v>
       </c>
       <c r="V18">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="10:23" x14ac:dyDescent="0.25">
@@ -897,10 +897,10 @@
         <v>4.5</v>
       </c>
       <c r="S19">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V19">
-        <v>12.85</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="20" spans="10:23" x14ac:dyDescent="0.25">
@@ -965,7 +965,7 @@
         <v>14.5</v>
       </c>
       <c r="S23">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="V23">
         <v>2</v>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="V29">
         <f>V18+V19+V20-V28+V23+V24-V27</f>
-        <v>-79.841724405821324</v>
+        <v>-97.191724405821319</v>
       </c>
       <c r="W29" t="s">
         <v>55</v>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="V32" s="3">
         <f>V29-V31</f>
-        <v>46.205726174475345</v>
+        <v>28.85572617447535</v>
       </c>
       <c r="W32" t="s">
         <v>56</v>
@@ -1226,9 +1226,6 @@
       <c r="V34">
         <f>2^($P11/($P$13*1000))-1</f>
         <v>0.3049549476889577</v>
-      </c>
-      <c r="W34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="35" spans="10:23" x14ac:dyDescent="0.25">
@@ -1288,7 +1285,7 @@
       </c>
       <c r="V37">
         <f>V32-V35</f>
-        <v>51.363369335607295</v>
+        <v>34.013369335607301</v>
       </c>
       <c r="W37" t="s">
         <v>56</v>
@@ -1342,7 +1339,7 @@
       </c>
       <c r="V41">
         <f>V32+10*LOG10($P13*1000/(V39))</f>
-        <v>50.362413930800038</v>
+        <v>33.012413930800044</v>
       </c>
       <c r="W41" t="s">
         <v>56</v>

</xml_diff>